<commit_message>
Mock Test document is in progress
Mock Test document is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6161FD8-4B82-41E6-9213-CD97510F7D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8285F2D4-3F6D-4399-8D10-32A6D48332E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpsTracker" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="75">
   <si>
     <t>Item Number</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Spoken English training to Victor</t>
   </si>
   <si>
-    <t>MS Office self training</t>
-  </si>
-  <si>
     <t>Teaching Ops training to team</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>Names</t>
   </si>
   <si>
-    <t>Anirban Chakroborty</t>
-  </si>
-  <si>
     <t>Student fees collection report</t>
   </si>
   <si>
@@ -197,9 +191,6 @@
     <t>Planned for 14-Nov After morning stand-up</t>
   </si>
   <si>
-    <t>Aniban to review the training plan by 10-Nov</t>
-  </si>
-  <si>
     <t>ID card for all</t>
   </si>
   <si>
@@ -239,13 +230,22 @@
     <t>Java Student Batch creation left</t>
   </si>
   <si>
-    <t>Debasish Sir left</t>
-  </si>
-  <si>
     <t>Electric Bill</t>
   </si>
   <si>
     <t>Pujo Subscription</t>
+  </si>
+  <si>
+    <t>Anirban Chakrabarty</t>
+  </si>
+  <si>
+    <t>MS Office training</t>
+  </si>
+  <si>
+    <t>ID card jacket purchase</t>
+  </si>
+  <si>
+    <t>Attendance Register</t>
   </si>
 </sst>
 </file>
@@ -635,25 +635,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.06640625" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -684,10 +683,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -701,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -715,7 +714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -729,10 +728,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -746,10 +745,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -764,7 +763,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -778,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -792,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -806,99 +805,96 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
       <c r="D12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -907,12 +903,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -921,12 +917,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -935,12 +931,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -949,12 +945,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -963,12 +959,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -977,141 +973,123 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F30" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Anirban"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Todo"/>
-        <filter val="WIP"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F30" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1121,226 +1099,226 @@
   <dimension ref="B2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B7" s="5" t="s">
+      <c r="C8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B9" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1350,39 +1328,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3518496C-1052-4545-B0C2-460165B8A9A2}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1391,12 +1369,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1405,88 +1383,116 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mock Test Student sheet created
Mock Test Student sheet created
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5339B6-7A78-4345-ADCF-4C1BD1020380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60933729-B7D9-47CF-AC63-066736CDF1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,15 +13,15 @@
     <sheet name="InternalAdmin" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">InternalAdmin!$A$1:$D$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OpsTracker!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">InternalAdmin!$A$1:$D$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OpsTracker!$A$1:$F$32</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="81">
   <si>
     <t>Item Number</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Buy JELET Book</t>
   </si>
   <si>
-    <t>Biscuits</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -257,7 +254,16 @@
     <t>Return of Merch (Debashish and Sayan)</t>
   </si>
   <si>
-    <t>Create a new Attendance Sheet</t>
+    <t>Book has to given to Avishek and Subroto Sir</t>
+  </si>
+  <si>
+    <t>Register for CRM information</t>
+  </si>
+  <si>
+    <t>Register for bio data of teacher</t>
+  </si>
+  <si>
+    <t>Organize the office different accessories</t>
   </si>
 </sst>
 </file>
@@ -647,11 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,7 +666,7 @@
     <col min="2" max="2" width="46.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -822,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -839,7 +845,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
         <v>53</v>
@@ -895,7 +901,7 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1007,13 +1013,13 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1052,7 +1058,7 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1072,7 +1078,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1088,13 +1094,16 @@
       <c r="D29" t="s">
         <v>10</v>
       </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1108,7 +1117,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
         <v>22</v>
@@ -1119,7 +1128,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>78</v>
@@ -1131,8 +1140,36 @@
         <v>6</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F30" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1184,7 +1221,7 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>51</v>
@@ -1371,11 +1408,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3518496C-1052-4545-B0C2-460165B8A9A2}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1473,13 +1510,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1501,10 +1538,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1518,10 +1555,10 @@
         <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1532,28 +1569,14 @@
         <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D9" xr:uid="{3518496C-1052-4545-B0C2-460165B8A9A2}"/>
+  <autoFilter ref="A1:D8" xr:uid="{3518496C-1052-4545-B0C2-460165B8A9A2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ops and Daily Status Updated
Ops and Daily Status Updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60933729-B7D9-47CF-AC63-066736CDF1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AF11F4-8280-48BE-82E9-FD600C7D3CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,14 +14,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">InternalAdmin!$A$1:$D$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OpsTracker!$A$1:$F$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OpsTracker!$A$1:$F$34</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="82">
   <si>
     <t>Item Number</t>
   </si>
@@ -257,13 +257,16 @@
     <t>Book has to given to Avishek and Subroto Sir</t>
   </si>
   <si>
-    <t>Register for CRM information</t>
-  </si>
-  <si>
-    <t>Register for bio data of teacher</t>
-  </si>
-  <si>
     <t>Organize the office different accessories</t>
+  </si>
+  <si>
+    <t>Online interview of Pronay Dhargave on 16 Nov at 3 PM</t>
+  </si>
+  <si>
+    <t>File for daily visit enquiry Sheet</t>
+  </si>
+  <si>
+    <t>File for bio data of teacher</t>
   </si>
 </sst>
 </file>
@@ -653,20 +656,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -918,7 +921,7 @@
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1131,7 +1134,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -1145,7 +1148,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -1159,7 +1162,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1168,8 +1171,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F34" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Daily Status updated in Mock Test Planning & Daily Status Tracker updated
Daily Status updated in Mock Test Planning & Daily Status Tracker updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85AEDF0-43AF-4A1E-8866-64FF4657F94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F18967-6636-45B9-B588-991E6C54EAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="96">
   <si>
     <t>Item Number</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Spoken English syllabus compilation</t>
   </si>
   <si>
-    <t>Spoken English training to Victor</t>
-  </si>
-  <si>
     <t>Teaching Ops training to team</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>Conduct Internal Assessment Test for existing Students</t>
   </si>
   <si>
-    <t>Java Student Batch creation left</t>
-  </si>
-  <si>
     <t>Electric Bill</t>
   </si>
   <si>
@@ -276,6 +270,45 @@
   </si>
   <si>
     <t>Need to take interview of Jayjit Sen on 16th Nov at 2 PM</t>
+  </si>
+  <si>
+    <t>Fees Collection report done.Java Student Batch creation left in ClassPlus APP</t>
+  </si>
+  <si>
+    <t>Start building up Mock Test Question Paper</t>
+  </si>
+  <si>
+    <t>Start building up Mock Test Presentation</t>
+  </si>
+  <si>
+    <t>Debashish To Help</t>
+  </si>
+  <si>
+    <t>Spoken English training to Victor &amp; Sathi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Tuesdays </t>
+  </si>
+  <si>
+    <t>Did not pick up the call..Need to call today</t>
+  </si>
+  <si>
+    <t>Three Mirrors. 1.5 Foot By 2 Foot</t>
+  </si>
+  <si>
+    <t>Phenyl</t>
+  </si>
+  <si>
+    <t>Switch Repair Kitchen</t>
+  </si>
+  <si>
+    <t>Light Point at Staircase</t>
+  </si>
+  <si>
+    <t>Tissue Paper dispensor at Bathroom in Ist Floor</t>
+  </si>
+  <si>
+    <t>Wet Tissue</t>
   </si>
 </sst>
 </file>
@@ -665,11 +698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +746,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -758,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -775,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -826,7 +859,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -834,19 +867,25 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
+      <c r="E10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -854,13 +893,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -868,13 +907,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -882,10 +921,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -896,13 +935,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -910,7 +949,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -924,13 +963,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -938,7 +977,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -952,7 +991,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -966,7 +1005,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -980,7 +1019,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -994,7 +1033,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1008,13 +1047,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1022,7 +1061,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1031,7 +1070,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1039,13 +1078,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1053,13 +1092,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1067,7 +1106,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1081,16 +1120,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1098,7 +1137,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1107,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1115,7 +1154,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1129,10 +1168,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -1143,7 +1182,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -1152,7 +1191,7 @@
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1160,7 +1199,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1169,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1177,10 +1216,10 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -1191,7 +1230,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -1205,13 +1244,50 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1241,210 +1317,210 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="G7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="I8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1454,17 +1530,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3518496C-1052-4545-B0C2-460165B8A9A2}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1472,13 +1548,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1500,7 +1576,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1514,13 +1590,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1528,13 +1604,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1542,13 +1618,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1556,13 +1632,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1570,13 +1646,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1584,13 +1660,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1598,10 +1674,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -1612,13 +1688,97 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mock Test Issues reverted by Waqar
Mock Test Issues reverted by Waqar
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3582D05-635E-4A9C-8768-9288BF008EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C488B1DD-2307-402A-84DA-11496FE6719B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="86">
   <si>
     <t>Item Number</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Sayan</t>
   </si>
   <si>
-    <t>Debasish</t>
-  </si>
-  <si>
     <t>Spoken English syllabus compilation</t>
   </si>
   <si>
@@ -276,6 +273,12 @@
   </si>
   <si>
     <t>Debashish and Ananya tested from our end and raised 25 defects. We notified College Doors</t>
+  </si>
+  <si>
+    <t>Prannay is selected.</t>
+  </si>
+  <si>
+    <t>Debashish</t>
   </si>
 </sst>
 </file>
@@ -666,7 +669,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +744,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -749,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -763,7 +766,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -772,7 +775,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -780,16 +783,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -797,10 +800,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -811,10 +814,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -825,7 +828,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -839,16 +842,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -856,10 +859,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -870,7 +873,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -884,7 +887,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -898,10 +901,10 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -912,10 +915,10 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -926,10 +929,10 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -940,16 +943,16 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -957,7 +960,7 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -971,16 +974,16 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -988,27 +991,27 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1016,10 +1019,10 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -1030,7 +1033,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -1039,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1047,7 +1050,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1056,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1064,13 +1067,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1078,7 +1084,7 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1087,7 +1093,7 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1095,7 +1101,7 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1104,7 +1110,7 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1112,16 +1118,16 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1129,16 +1135,16 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1168,210 +1174,210 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="G7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="I8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1399,13 +1405,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1413,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1427,13 +1433,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1441,13 +1447,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1455,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1469,13 +1475,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1483,13 +1489,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1497,13 +1503,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1511,13 +1517,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1525,13 +1531,13 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1539,13 +1545,13 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1553,13 +1559,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1567,13 +1573,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily Status Tracker and Ops updated
Daily Status Tracker and Ops updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/Ops/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD2AD58-8A94-43CF-B7FF-7104ECEF1884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931340DC-01E6-4A9E-A3C6-B94EFA4B2FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">InternalAdmin!$A$1:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OpsTracker!$A$1:$F$75</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -228,9 +239,6 @@
 Waqar reverted back and we will check on Monday (20th November 2023)</t>
   </si>
   <si>
-    <t>Subroto Sir will set Question paper by Thursday (23-11-2023)</t>
-  </si>
-  <si>
     <t>Conduct Internal Assessment Test Physics</t>
   </si>
   <si>
@@ -411,10 +419,13 @@
     <t>Talk to Avishek Sir.  Talked with Avishek Sir. He will take test on 25-11-2023.</t>
   </si>
   <si>
-    <t>Prannay is selected. His biodata has ben taken.AADHAR card needs to be taken.</t>
-  </si>
-  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Prannay is selected. His biodata and AADHAR card has been collected.</t>
+  </si>
+  <si>
+    <t>Subroto Sir will set question paper.</t>
   </si>
 </sst>
 </file>
@@ -820,7 +831,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,7 +906,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1047,7 +1058,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1055,7 +1066,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
         <v>65</v>
@@ -1064,7 +1075,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1072,7 +1083,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>65</v>
@@ -1081,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
@@ -1143,7 +1154,7 @@
         <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E20" t="s">
         <v>129</v>
@@ -1154,16 +1165,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" t="s">
-        <v>75</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
@@ -1171,7 +1182,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1180,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
@@ -1219,7 +1230,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1228,7 +1239,7 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
@@ -1236,7 +1247,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1287,7 +1298,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
@@ -1295,7 +1306,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
@@ -1303,7 +1314,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
@@ -1311,7 +1322,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1319,7 +1330,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1327,7 +1338,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1335,7 +1346,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1343,7 +1354,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1351,7 +1362,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1359,7 +1370,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1367,7 +1378,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1375,7 +1386,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1383,7 +1394,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1391,7 +1402,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1399,7 +1410,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1407,7 +1418,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1415,7 +1426,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1423,7 +1434,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1431,7 +1442,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1439,7 +1450,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1458,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1455,7 +1466,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1463,7 +1474,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1471,7 +1482,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1479,7 +1490,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1487,7 +1498,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1495,7 +1506,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1503,7 +1514,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1511,7 +1522,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1519,7 +1530,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1527,7 +1538,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1535,7 +1546,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1543,7 +1554,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1551,7 +1562,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1559,7 +1570,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1567,7 +1578,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1575,7 +1586,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1583,7 +1594,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1591,7 +1602,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1599,7 +1610,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1607,7 +1618,7 @@
         <v>69</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1615,7 +1626,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1623,7 +1634,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1631,7 +1642,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1639,7 +1650,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1647,7 +1658,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -1655,7 +1666,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>